<commit_message>
add cart, order and courier api
</commit_message>
<xml_diff>
--- a/resources/imports/OrderSeeder.xlsx
+++ b/resources/imports/OrderSeeder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kampus\Perkuliahan\Semester 4\Pemrograman Web\Proyek Akhir\source\mlijo-apps\resources\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC27EC16-1793-44EF-B61A-B00A8611B9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E29BDE-68BE-4734-97D4-54D15D689F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33255" yWindow="2595" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33330" yWindow="2235" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>processing</t>
   </si>
   <si>
-    <t>Transaksi Berahasil Dibuat</t>
-  </si>
-  <si>
     <t>Transaksi Dalam Proses</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>INV2022050100011</t>
+  </si>
+  <si>
+    <t>Transaksi Berhasil Dibuat</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="3"/>
       <c r="I2" s="5"/>
@@ -726,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" t="s">
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="3"/>
       <c r="I4" s="5"/>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>29</v>
@@ -849,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="4"/>
       <c r="I6" s="5"/>
@@ -886,7 +886,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="3"/>
       <c r="I7" s="5"/>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>30</v>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="3"/>
       <c r="I9" s="5"/>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" s="3"/>
       <c r="I10" s="5"/>
@@ -1041,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" s="6"/>
       <c r="I11" s="5"/>
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0394368F-9D83-4DEB-944E-07C607BF6285}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1097,10 +1097,10 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -1144,7 +1144,7 @@
         <v>34000</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>3920</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>14000</v>
@@ -1277,7 +1277,7 @@
         <v>23000</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C29544-2D83-41A8-B75D-76ADFB18FA74}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,7 +1562,7 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,7 +1688,7 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
         <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1716,7 +1716,7 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1780,19 +1780,19 @@
         <v>85637263561</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2">
         <v>68462</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,19 +1806,19 @@
         <v>85637263561</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3">
         <v>68462</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1832,19 +1832,19 @@
         <v>85637263561</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4">
         <v>68462</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1858,19 +1858,19 @@
         <v>85637263561</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5">
         <v>68462</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1884,19 +1884,19 @@
         <v>85637263562</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6">
         <v>68462</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1910,19 +1910,19 @@
         <v>85637263563</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7">
         <v>68462</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1936,19 +1936,19 @@
         <v>85637263564</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8">
         <v>68462</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1962,19 +1962,19 @@
         <v>85637263564</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9">
         <v>68462</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1988,19 +1988,19 @@
         <v>85637263564</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10">
         <v>68462</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2014,19 +2014,19 @@
         <v>85637263565</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11">
         <v>68462</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>